<commit_message>
Change field names in the "Indices" sheet
</commit_message>
<xml_diff>
--- a/Mapas_ES/Dados/divisoes_administrativas_ES.xlsx
+++ b/Mapas_ES/Dados/divisoes_administrativas_ES.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fcsardinha\OneDrive - Secretaria de Estado da Educação\Documentos\Projetos\Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A58D430-0283-41E8-8C57-7D442F871ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F7F413-41EE-4816-B84B-F94574318644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Divisoes" sheetId="2" r:id="rId1"/>
     <sheet name="Indices" sheetId="6" r:id="rId2"/>
-    <sheet name="Calculos" sheetId="3" r:id="rId3"/>
-    <sheet name="IBGE-JUN2025" sheetId="4" r:id="rId4"/>
-    <sheet name="Rural-Urbano" sheetId="5" r:id="rId5"/>
+    <sheet name="Notas_Indices" sheetId="7" r:id="rId3"/>
+    <sheet name="Calculos" sheetId="3" r:id="rId4"/>
+    <sheet name="IBGE-JUN2025" sheetId="4" r:id="rId5"/>
+    <sheet name="Rural-Urbano" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Calculos!$A$1:$H$79</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Calculos!$A$1:$H$79</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Divisoes!$A$1:$K$79</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Indices!$A$1:$G$79</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Indices!$A$1:$H$79</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1517" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1517" uniqueCount="446">
   <si>
     <t>LATITUDE_MUN</t>
   </si>
@@ -1352,9 +1353,6 @@
     <t>Nota 3 - A nova classificação do IBGE propõe uma visão mais detalhada da ruralidade, com diferentes tipos de espaços rurais, incluindo:</t>
   </si>
   <si>
-    <t>IDHM [2010]</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nota 4 - IDHM = Índice de Desenvolvimento Humano Municipal [2010] é um índice que mede o grau de desenvolvimento humano em nível municipal, </t>
   </si>
   <si>
@@ -1365,6 +1363,27 @@
   </si>
   <si>
     <t>Densidade demográfica - hab/km² [Calculada]</t>
+  </si>
+  <si>
+    <t>Nota 3 - Tipologia Rural-Urbana (IBGE) - A nova classificação do IBGE propõe uma visão mais detalhada da ruralidade, com diferentes tipos de espaços rurais, incluindo:</t>
+  </si>
+  <si>
+    <t>TIPO_RURAL_URBANO</t>
+  </si>
+  <si>
+    <t>AREA_MUN</t>
+  </si>
+  <si>
+    <t>POPULACAO_MUN</t>
+  </si>
+  <si>
+    <t>DENS_DEMOG_MUN</t>
+  </si>
+  <si>
+    <t>IDHM</t>
+  </si>
+  <si>
+    <t>Nota 2 - Porte Populacional - Municípios com:</t>
   </si>
 </sst>
 </file>
@@ -1373,7 +1392,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -1409,7 +1428,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -4482,22 +4501,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E17A431-8B28-46E1-AA6C-9C27CAA71A50}">
-  <dimension ref="A1:H95"/>
+  <dimension ref="A1:H79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="5" customWidth="1"/>
     <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -4508,22 +4527,22 @@
         <v>176</v>
       </c>
       <c r="C1" t="s">
-        <v>428</v>
+        <v>440</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>197</v>
+        <v>441</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>198</v>
+        <v>442</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>199</v>
+        <v>443</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>180</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -6554,79 +6573,105 @@
         <v>0.84499999999999997</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="5" t="s">
+  </sheetData>
+  <autoFilter ref="A1:H79" xr:uid="{5E17A431-8B28-46E1-AA6C-9C27CAA71A50}"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDA242A6-9B0F-4725-A738-16893D000E4C}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="5" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B84" s="2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="2" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B86" s="2" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B87" s="2" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="5" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B90" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="5" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" t="s">
         <v>437</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B95" t="s">
-        <v>438</v>
       </c>
     </row>
   </sheetData>
@@ -6634,7 +6679,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40CCBB74-AE0C-4775-8892-75B1737676A0}">
   <dimension ref="A1:I95"/>
   <sheetViews>
@@ -6672,7 +6717,7 @@
         <v>199</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>185</v>
@@ -9161,17 +9206,17 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
   </sheetData>
@@ -9179,7 +9224,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E05A355C-DF46-4416-87E8-005286907734}">
   <dimension ref="A1:O94"/>
   <sheetViews>
@@ -12982,11 +13027,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{740800BB-FE9C-4A8E-9F13-1F8E0163CEDC}">
   <dimension ref="A1:G85"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B81" sqref="B81:B85"/>
     </sheetView>
   </sheetViews>

</xml_diff>